<commit_message>
requirements y README actualizado.
</commit_message>
<xml_diff>
--- a/data/templates.xlsx
+++ b/data/templates.xlsx
@@ -1322,7 +1322,7 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>Acero</t>
+          <t>Vidrio</t>
         </is>
       </c>
       <c r="D2" s="3" t="n"/>
@@ -1362,7 +1362,7 @@
         </is>
       </c>
       <c r="C3" s="3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D3" s="3" t="n"/>
       <c r="E3" s="3" t="n"/>
@@ -1440,7 +1440,7 @@
         </is>
       </c>
       <c r="C5" s="3" t="n">
-        <v>0.3</v>
+        <v>0.008</v>
       </c>
       <c r="D5" s="3" t="n"/>
       <c r="E5" s="3" t="n"/>
@@ -1479,7 +1479,7 @@
         </is>
       </c>
       <c r="C6" s="3" t="n">
-        <v>40</v>
+        <v>1512</v>
       </c>
       <c r="D6" s="3" t="n"/>
       <c r="E6" s="3" t="n"/>
@@ -1652,97 +1652,97 @@
         </is>
       </c>
       <c r="C9" s="7" t="n">
-        <v>46.29</v>
+        <v>5.04</v>
       </c>
       <c r="D9" s="5" t="n">
-        <v>48.23</v>
+        <v>6.98</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>50.24</v>
+        <v>8.99</v>
       </c>
       <c r="F9" s="5" t="n">
-        <v>47.56</v>
+        <v>11.06</v>
       </c>
       <c r="G9" s="5" t="n">
-        <v>52.69</v>
+        <v>13</v>
       </c>
       <c r="H9" s="5" t="n">
-        <v>56.65</v>
+        <v>15.01</v>
       </c>
       <c r="I9" s="5" t="n">
-        <v>59.86</v>
+        <v>17.08</v>
       </c>
       <c r="J9" s="5" t="n">
-        <v>62.83</v>
+        <v>19.02</v>
       </c>
       <c r="K9" s="5" t="n">
-        <v>65.93000000000001</v>
+        <v>20.96</v>
       </c>
       <c r="L9" s="5" t="n">
-        <v>68.64</v>
+        <v>23.1</v>
       </c>
       <c r="M9" s="5" t="n">
-        <v>71.27</v>
+        <v>25.04</v>
       </c>
       <c r="N9" s="5" t="n">
-        <v>73.95</v>
+        <v>26.98</v>
       </c>
       <c r="O9" s="5" t="n">
-        <v>76.68000000000001</v>
+        <v>28.99</v>
       </c>
       <c r="P9" s="5" t="n">
-        <v>79.19</v>
+        <v>31.06</v>
       </c>
       <c r="Q9" s="5" t="n">
-        <v>81.78</v>
+        <v>33</v>
       </c>
       <c r="R9" s="5" t="n">
-        <v>84.44</v>
+        <v>35.01</v>
       </c>
       <c r="S9" s="6" t="n">
-        <v>86.91</v>
+        <v>37.08</v>
       </c>
       <c r="T9" s="5" t="n">
-        <v>89.36</v>
+        <v>39.02</v>
       </c>
       <c r="U9" s="5" t="n">
-        <v>92.08</v>
+        <v>40.96</v>
       </c>
       <c r="V9" s="5" t="n">
-        <v>94.52</v>
+        <v>15.03</v>
       </c>
       <c r="W9" s="5" t="n">
-        <v>96.95999999999999</v>
+        <v>24.39</v>
       </c>
       <c r="X9" s="5" t="n">
-        <v>99.48999999999999</v>
+        <v>29.37</v>
       </c>
       <c r="Y9" s="5" t="n">
-        <v>102.09</v>
+        <v>33.55</v>
       </c>
       <c r="Z9" s="5" t="n">
-        <v>104.53</v>
+        <v>37.42</v>
       </c>
       <c r="AA9" s="5" t="n">
-        <v>107.04</v>
+        <v>40.81</v>
       </c>
       <c r="AB9" s="5" t="n">
-        <v>109.64</v>
+        <v>44.18</v>
       </c>
       <c r="AC9" s="5" t="n">
-        <v>100.27</v>
+        <v>47.57</v>
       </c>
       <c r="AD9" s="5" t="n">
-        <v>102.21</v>
+        <v>50.66</v>
       </c>
       <c r="AE9" s="5" t="n">
-        <v>104.35</v>
+        <v>53.71</v>
       </c>
       <c r="AF9" s="5" t="n">
-        <v>106.29</v>
+        <v>57.05</v>
       </c>
       <c r="AG9" s="5" t="n">
-        <v/>
+        <v>60.04</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1">
@@ -1752,97 +1752,97 @@
         </is>
       </c>
       <c r="C10" s="5" t="n">
-        <v>55.2</v>
+        <v>12.5</v>
       </c>
       <c r="D10" s="5" t="n">
-        <v>55.1</v>
+        <v>12.9</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>55.6</v>
+        <v>13.7</v>
       </c>
       <c r="F10" s="5" t="n">
-        <v>57.7</v>
+        <v>14.8</v>
       </c>
       <c r="G10" s="5" t="n">
-        <v>63</v>
+        <v>15.9</v>
       </c>
       <c r="H10" s="5" t="n">
-        <v>62.5</v>
+        <v>17.2</v>
       </c>
       <c r="I10" s="5" t="n">
-        <v>63</v>
+        <v>18.6</v>
       </c>
       <c r="J10" s="5" t="n">
-        <v>63.3</v>
+        <v>20</v>
       </c>
       <c r="K10" s="5" t="n">
-        <v>64.8</v>
+        <v>21.4</v>
       </c>
       <c r="L10" s="5" t="n">
-        <v>67.8</v>
+        <v>23</v>
       </c>
       <c r="M10" s="5" t="n">
-        <v>70.40000000000001</v>
+        <v>24.5</v>
       </c>
       <c r="N10" s="5" t="n">
-        <v>72.90000000000001</v>
+        <v>25.9</v>
       </c>
       <c r="O10" s="5" t="n">
-        <v>75.5</v>
+        <v>27.4</v>
       </c>
       <c r="P10" s="5" t="n">
-        <v>78.09999999999999</v>
+        <v>28.9</v>
       </c>
       <c r="Q10" s="5" t="n">
-        <v>80.5</v>
+        <v>30.2</v>
       </c>
       <c r="R10" s="5" t="n">
-        <v>83</v>
+        <v>31.4</v>
       </c>
       <c r="S10" s="6" t="n">
-        <v>85.40000000000001</v>
+        <v>32.3</v>
       </c>
       <c r="T10" s="5" t="n">
-        <v>87.7</v>
+        <v>32.7</v>
       </c>
       <c r="U10" s="5" t="n">
-        <v>89.90000000000001</v>
+        <v>31.7</v>
       </c>
       <c r="V10" s="5" t="n">
-        <v>92.2</v>
+        <v>22.1</v>
       </c>
       <c r="W10" s="5" t="n">
-        <v>94.2</v>
+        <v>27.4</v>
       </c>
       <c r="X10" s="5" t="n">
-        <v>96.2</v>
+        <v>31.9</v>
       </c>
       <c r="Y10" s="5" t="n">
-        <v>98.09999999999999</v>
+        <v>35.8</v>
       </c>
       <c r="Z10" s="5" t="n">
-        <v>99.90000000000001</v>
+        <v>39.5</v>
       </c>
       <c r="AA10" s="5" t="n">
-        <v>101.4</v>
+        <v>42.8</v>
       </c>
       <c r="AB10" s="5" t="n">
-        <v>102.9</v>
+        <v>46.1</v>
       </c>
       <c r="AC10" s="5" t="n">
-        <v>104.4</v>
+        <v>49.4</v>
       </c>
       <c r="AD10" s="5" t="n">
-        <v>105.8</v>
+        <v>52.4</v>
       </c>
       <c r="AE10" s="5" t="n">
-        <v>107.1</v>
+        <v>55.3</v>
       </c>
       <c r="AF10" s="5" t="n">
-        <v>108.6</v>
+        <v>58.5</v>
       </c>
       <c r="AG10" s="5" t="n">
-        <v>110</v>
+        <v>61.4</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1">
@@ -1852,97 +1852,97 @@
         </is>
       </c>
       <c r="C11" s="5" t="n">
-        <v>51.61</v>
+        <v>4.77</v>
       </c>
       <c r="D11" s="5" t="n">
-        <v>53.55</v>
+        <v>6.56</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>55.56</v>
+        <v>8.460000000000001</v>
       </c>
       <c r="F11" s="5" t="n">
-        <v>57.63</v>
+        <v>10.47</v>
       </c>
       <c r="G11" s="5" t="n">
-        <v>59.57</v>
+        <v>12.37</v>
       </c>
       <c r="H11" s="5" t="n">
-        <v>61.51</v>
+        <v>14.35</v>
       </c>
       <c r="I11" s="5" t="n">
-        <v>63.65</v>
+        <v>16.41</v>
       </c>
       <c r="J11" s="5" t="n">
-        <v>65.59</v>
+        <v>18.34</v>
       </c>
       <c r="K11" s="5" t="n">
-        <v>67.53</v>
+        <v>20.27</v>
       </c>
       <c r="L11" s="5" t="n">
-        <v>69.54000000000001</v>
+        <v>22.41</v>
       </c>
       <c r="M11" s="5" t="n">
-        <v>71.61</v>
+        <v>24.35</v>
       </c>
       <c r="N11" s="5" t="n">
-        <v>73.55</v>
+        <v>26.28</v>
       </c>
       <c r="O11" s="5" t="n">
-        <v>75.56</v>
+        <v>28.29</v>
       </c>
       <c r="P11" s="5" t="n">
-        <v>77.63</v>
+        <v>30.36</v>
       </c>
       <c r="Q11" s="5" t="n">
-        <v>79.56999999999999</v>
+        <v>32.3</v>
       </c>
       <c r="R11" s="5" t="n">
-        <v>81.51000000000001</v>
+        <v>34.31</v>
       </c>
       <c r="S11" s="6" t="n">
-        <v>83.65000000000001</v>
+        <v>33.45</v>
       </c>
       <c r="T11" s="5" t="n">
-        <v>85.59</v>
+        <v>32.44</v>
       </c>
       <c r="U11" s="5" t="n">
-        <v>87.53</v>
+        <v>31.18</v>
       </c>
       <c r="V11" s="5" t="n">
-        <v>89.54000000000001</v>
+        <v>29.42</v>
       </c>
       <c r="W11" s="5" t="n">
-        <v>91.61</v>
+        <v>32.3</v>
       </c>
       <c r="X11" s="5" t="n">
-        <v>93.55</v>
+        <v>35.19</v>
       </c>
       <c r="Y11" s="5" t="n">
-        <v>95.56</v>
+        <v>38.18</v>
       </c>
       <c r="Z11" s="5" t="n">
-        <v>97.63</v>
+        <v>41.27</v>
       </c>
       <c r="AA11" s="5" t="n">
-        <v>99.56999999999999</v>
+        <v>44.17</v>
       </c>
       <c r="AB11" s="5" t="n">
-        <v>101.51</v>
+        <v>47.17</v>
       </c>
       <c r="AC11" s="5" t="n">
-        <v>103.65</v>
+        <v>50.27</v>
       </c>
       <c r="AD11" s="5" t="n">
-        <v>105.59</v>
+        <v>53.16</v>
       </c>
       <c r="AE11" s="5" t="n">
-        <v/>
+        <v>56.06</v>
       </c>
       <c r="AF11" s="5" t="n">
-        <v/>
+        <v>59.27</v>
       </c>
       <c r="AG11" s="5" t="n">
-        <v/>
+        <v>62.17</v>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1">
@@ -1952,97 +1952,97 @@
         </is>
       </c>
       <c r="C12" s="5" t="n">
-        <v>52.56</v>
+        <v>10.78</v>
       </c>
       <c r="D12" s="5" t="n">
-        <v>52.6</v>
+        <v>11.7</v>
       </c>
       <c r="E12" s="5" t="n">
-        <v>52.52</v>
+        <v>12.83</v>
       </c>
       <c r="F12" s="5" t="n">
-        <v>58.28</v>
+        <v>14.16</v>
       </c>
       <c r="G12" s="5" t="n">
-        <v>59.74</v>
+        <v>15.49</v>
       </c>
       <c r="H12" s="5" t="n">
-        <v>61.24</v>
+        <v>16.95</v>
       </c>
       <c r="I12" s="5" t="n">
-        <v>62.8</v>
+        <v>18.52</v>
       </c>
       <c r="J12" s="5" t="n">
-        <v>64.25</v>
+        <v>20.03</v>
       </c>
       <c r="K12" s="5" t="n">
-        <v>65.7</v>
+        <v>21.58</v>
       </c>
       <c r="L12" s="5" t="n">
-        <v>67.72</v>
+        <v>23.33</v>
       </c>
       <c r="M12" s="5" t="n">
-        <v>70.43000000000001</v>
+        <v>24.94</v>
       </c>
       <c r="N12" s="5" t="n">
-        <v>73.06</v>
+        <v>26.57</v>
       </c>
       <c r="O12" s="5" t="n">
-        <v>75.73999999999999</v>
+        <v>28.28</v>
       </c>
       <c r="P12" s="5" t="n">
-        <v>78.45999999999999</v>
+        <v>30.06</v>
       </c>
       <c r="Q12" s="5" t="n">
-        <v>80.98</v>
+        <v>31.74</v>
       </c>
       <c r="R12" s="5" t="n">
-        <v>83.56999999999999</v>
+        <v>33.48</v>
       </c>
       <c r="S12" s="6" t="n">
-        <v>86.23</v>
+        <v>35.25</v>
       </c>
       <c r="T12" s="5" t="n">
-        <v>88.69</v>
+        <v>36.79</v>
       </c>
       <c r="U12" s="5" t="n">
-        <v>91.15000000000001</v>
+        <v>37.17</v>
       </c>
       <c r="V12" s="5" t="n">
-        <v>93.87</v>
+        <v>23.39</v>
       </c>
       <c r="W12" s="5" t="n">
-        <v>96.31</v>
+        <v>26.28</v>
       </c>
       <c r="X12" s="5" t="n">
-        <v>98.75</v>
+        <v>31.16</v>
       </c>
       <c r="Y12" s="5" t="n">
-        <v>101.28</v>
+        <v>35.34</v>
       </c>
       <c r="Z12" s="5" t="n">
-        <v>103.88</v>
+        <v>39.21</v>
       </c>
       <c r="AA12" s="5" t="n">
-        <v>106.31</v>
+        <v>42.6</v>
       </c>
       <c r="AB12" s="5" t="n">
-        <v>108.83</v>
+        <v>45.97</v>
       </c>
       <c r="AC12" s="5" t="n">
-        <v>111.43</v>
+        <v>49.36</v>
       </c>
       <c r="AD12" s="5" t="n">
-        <v>113.86</v>
+        <v>52.45</v>
       </c>
       <c r="AE12" s="5" t="n">
-        <v>116.29</v>
+        <v>55.5</v>
       </c>
       <c r="AF12" s="5" t="n">
-        <v>118.97</v>
+        <v>58.84</v>
       </c>
       <c r="AG12" s="5" t="n">
-        <v>121.4</v>
+        <v>61.83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>